<commit_message>
add platform column for lambrechts_2018_6653
</commit_message>
<xml_diff>
--- a/pipeline_stages/00_process_fastq/lambrechts_2018_6653/samples.xlsx
+++ b/pipeline_stages/00_process_fastq/lambrechts_2018_6653/samples.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="243">
   <si>
     <t xml:space="preserve">samples</t>
   </si>
@@ -50,6 +50,9 @@
     <t xml:space="preserve">tumor_type</t>
   </si>
   <si>
+    <t xml:space="preserve">platform</t>
+  </si>
+  <si>
     <t xml:space="preserve">age</t>
   </si>
   <si>
@@ -66,6 +69,9 @@
   </si>
   <si>
     <t xml:space="preserve">LUAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10x_3p_v2</t>
   </si>
   <si>
     <t xml:space="preserve">male</t>
@@ -848,7 +854,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -912,10 +918,13 @@
       <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>10000</v>
@@ -930,27 +939,30 @@
         <v>6</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="K2" s="0" t="s">
-        <v>15</v>
+      <c r="L2" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>10000</v>
@@ -965,28 +977,31 @@
         <v>6</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="K3" s="0" t="s">
-        <v>15</v>
+      <c r="L3" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="M3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>10000</v>
@@ -1001,28 +1016,31 @@
         <v>6</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="K4" s="0" t="s">
-        <v>15</v>
+      <c r="L4" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="M4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>10000</v>
@@ -1037,28 +1055,31 @@
         <v>6</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="K5" s="0" t="s">
-        <v>15</v>
+      <c r="L5" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="M5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>10000</v>
@@ -1073,28 +1094,31 @@
         <v>7</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="K6" s="0" t="s">
-        <v>15</v>
+      <c r="L6" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="M6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>10000</v>
@@ -1109,28 +1133,31 @@
         <v>7</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="K7" s="0" t="s">
-        <v>15</v>
+      <c r="L7" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="M7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>10000</v>
@@ -1145,28 +1172,31 @@
         <v>7</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="K8" s="0" t="s">
-        <v>15</v>
+      <c r="L8" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="M8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>10000</v>
@@ -1181,28 +1211,31 @@
         <v>7</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="K9" s="0" t="s">
-        <v>15</v>
+      <c r="L9" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="M9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>10000</v>
@@ -1217,28 +1250,31 @@
         <v>8</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="K10" s="0" t="s">
-        <v>26</v>
+      <c r="L10" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="M10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>10000</v>
@@ -1253,28 +1289,31 @@
         <v>8</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="K11" s="0" t="s">
-        <v>26</v>
+      <c r="L11" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="M11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>10000</v>
@@ -1289,28 +1328,31 @@
         <v>8</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="K12" s="0" t="s">
-        <v>26</v>
+      <c r="L12" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="M12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>10000</v>
@@ -1325,22 +1367,25 @@
         <v>8</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="K13" s="0" t="s">
-        <v>26</v>
+      <c r="L13" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="M13" s="1"/>
     </row>
@@ -1366,12 +1411,12 @@
   <dimension ref="A1:BF13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="1" sqref="J3:J13 C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16"/>
@@ -1401,166 +1446,166 @@
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Z1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF1" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG1" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH1" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB1" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC1" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD1" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE1" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF1" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG1" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH1" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="AI1" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AY1" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AZ1" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="BB1" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="BC1" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="BD1" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="BE1" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="BF1" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1575,19 +1620,19 @@
         <v>98</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>6</v>
@@ -1596,64 +1641,64 @@
         <v>65</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AD2" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AE2" s="0" t="n">
         <v>88</v>
@@ -1662,37 +1707,37 @@
         <v>0</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AJ2" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="AK2" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AM2" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="AN2" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="AO2" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="AP2" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="AQ2" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="AR2" s="0" t="n">
         <v>912</v>
@@ -1701,13 +1746,13 @@
         <v>457</v>
       </c>
       <c r="AT2" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="AU2" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="AV2" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AW2" s="0" t="n">
         <v>14</v>
@@ -1716,7 +1761,7 @@
         <v>10</v>
       </c>
       <c r="AY2" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AZ2" s="0" t="n">
         <v>0</v>
@@ -1725,7 +1770,7 @@
         <v>14</v>
       </c>
       <c r="BB2" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="BC2" s="0" t="n">
         <v>0</v>
@@ -1737,7 +1782,7 @@
         <v>6</v>
       </c>
       <c r="BF2" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1752,19 +1797,19 @@
         <v>98</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>6</v>
@@ -1773,64 +1818,64 @@
         <v>65</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AA3" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AC3" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AD3" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AE3" s="0" t="n">
         <v>88</v>
@@ -1839,37 +1884,37 @@
         <v>0</v>
       </c>
       <c r="AG3" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AH3" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AI3" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AJ3" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="AK3" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AL3" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="AM3" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="AN3" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="AO3" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AP3" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="AQ3" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="AR3" s="0" t="n">
         <v>914</v>
@@ -1878,13 +1923,13 @@
         <v>458</v>
       </c>
       <c r="AT3" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="AU3" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AV3" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AW3" s="0" t="n">
         <v>14</v>
@@ -1893,7 +1938,7 @@
         <v>10</v>
       </c>
       <c r="AY3" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AZ3" s="0" t="n">
         <v>0</v>
@@ -1902,7 +1947,7 @@
         <v>14</v>
       </c>
       <c r="BB3" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="BC3" s="0" t="n">
         <v>0</v>
@@ -1914,7 +1959,7 @@
         <v>6</v>
       </c>
       <c r="BF3" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1929,19 +1974,19 @@
         <v>98</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>6</v>
@@ -1950,64 +1995,64 @@
         <v>65</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="V4" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Y4" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AA4" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB4" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AC4" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AD4" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AE4" s="0" t="n">
         <v>88</v>
@@ -2016,37 +2061,37 @@
         <v>0</v>
       </c>
       <c r="AG4" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AH4" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AI4" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AJ4" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AK4" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AL4" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="AM4" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AN4" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AO4" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AP4" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AQ4" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AR4" s="0" t="n">
         <v>912</v>
@@ -2055,13 +2100,13 @@
         <v>457</v>
       </c>
       <c r="AT4" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AU4" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AV4" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AW4" s="0" t="n">
         <v>14</v>
@@ -2070,7 +2115,7 @@
         <v>10</v>
       </c>
       <c r="AY4" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AZ4" s="0" t="n">
         <v>0</v>
@@ -2079,7 +2124,7 @@
         <v>14</v>
       </c>
       <c r="BB4" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="BC4" s="0" t="n">
         <v>0</v>
@@ -2091,7 +2136,7 @@
         <v>6</v>
       </c>
       <c r="BF4" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,19 +2151,19 @@
         <v>98</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>6</v>
@@ -2127,64 +2172,64 @@
         <v>65</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="V5" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Y5" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AA5" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB5" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AC5" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AD5" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AE5" s="0" t="n">
         <v>88</v>
@@ -2193,37 +2238,37 @@
         <v>0</v>
       </c>
       <c r="AG5" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AH5" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AI5" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AJ5" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AK5" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AL5" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AM5" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AN5" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AO5" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AP5" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AQ5" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AR5" s="0" t="n">
         <v>914</v>
@@ -2232,13 +2277,13 @@
         <v>458</v>
       </c>
       <c r="AT5" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="AU5" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AV5" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AW5" s="0" t="n">
         <v>14</v>
@@ -2247,7 +2292,7 @@
         <v>10</v>
       </c>
       <c r="AY5" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AZ5" s="0" t="n">
         <v>0</v>
@@ -2256,7 +2301,7 @@
         <v>14</v>
       </c>
       <c r="BB5" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="BC5" s="0" t="n">
         <v>0</v>
@@ -2268,7 +2313,7 @@
         <v>6</v>
       </c>
       <c r="BF5" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2283,19 +2328,19 @@
         <v>88</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>7</v>
@@ -2304,64 +2349,64 @@
         <v>60</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="V6" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="W6" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Y6" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="Z6" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AA6" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB6" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AC6" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AD6" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AE6" s="0" t="n">
         <v>88</v>
@@ -2370,37 +2415,37 @@
         <v>0</v>
       </c>
       <c r="AG6" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AH6" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AI6" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AJ6" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="AK6" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AL6" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="AM6" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="AN6" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="AO6" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="AP6" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AQ6" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="AR6" s="0" t="n">
         <v>850</v>
@@ -2409,13 +2454,13 @@
         <v>426</v>
       </c>
       <c r="AT6" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="AU6" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="AV6" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AW6" s="0" t="n">
         <v>14</v>
@@ -2424,7 +2469,7 @@
         <v>10</v>
       </c>
       <c r="AY6" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AZ6" s="0" t="n">
         <v>0</v>
@@ -2433,7 +2478,7 @@
         <v>14</v>
       </c>
       <c r="BB6" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="BC6" s="0" t="n">
         <v>0</v>
@@ -2445,7 +2490,7 @@
         <v>7</v>
       </c>
       <c r="BF6" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2460,19 +2505,19 @@
         <v>88</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>7</v>
@@ -2481,64 +2526,64 @@
         <v>60</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="T7" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="U7" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="V7" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="W7" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="X7" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Y7" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="Z7" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AA7" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB7" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AC7" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AD7" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AE7" s="0" t="n">
         <v>88</v>
@@ -2547,37 +2592,37 @@
         <v>0</v>
       </c>
       <c r="AG7" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AH7" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AI7" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AJ7" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="AK7" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AL7" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="AM7" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="AN7" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="AO7" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="AP7" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="AQ7" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AR7" s="0" t="n">
         <v>850</v>
@@ -2586,13 +2631,13 @@
         <v>426</v>
       </c>
       <c r="AT7" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AU7" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AV7" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AW7" s="0" t="n">
         <v>14</v>
@@ -2601,7 +2646,7 @@
         <v>10</v>
       </c>
       <c r="AY7" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AZ7" s="0" t="n">
         <v>0</v>
@@ -2610,7 +2655,7 @@
         <v>14</v>
       </c>
       <c r="BB7" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="BC7" s="0" t="n">
         <v>0</v>
@@ -2622,7 +2667,7 @@
         <v>7</v>
       </c>
       <c r="BF7" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2637,19 +2682,19 @@
         <v>88</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>7</v>
@@ -2658,64 +2703,64 @@
         <v>60</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="T8" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="V8" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="X8" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Y8" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AA8" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB8" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AC8" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AD8" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AE8" s="0" t="n">
         <v>88</v>
@@ -2724,37 +2769,37 @@
         <v>0</v>
       </c>
       <c r="AG8" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AH8" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AI8" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AJ8" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="AK8" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AL8" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AM8" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AN8" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="AO8" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="AP8" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="AQ8" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="AR8" s="0" t="n">
         <v>850</v>
@@ -2763,13 +2808,13 @@
         <v>426</v>
       </c>
       <c r="AT8" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="AU8" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="AV8" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AW8" s="0" t="n">
         <v>14</v>
@@ -2778,7 +2823,7 @@
         <v>10</v>
       </c>
       <c r="AY8" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AZ8" s="0" t="n">
         <v>0</v>
@@ -2787,7 +2832,7 @@
         <v>14</v>
       </c>
       <c r="BB8" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="BC8" s="0" t="n">
         <v>0</v>
@@ -2799,7 +2844,7 @@
         <v>7</v>
       </c>
       <c r="BF8" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2814,19 +2859,19 @@
         <v>88</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>7</v>
@@ -2835,64 +2880,64 @@
         <v>60</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="T9" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="U9" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="V9" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="X9" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Y9" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="Z9" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AA9" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB9" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AC9" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AD9" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AE9" s="0" t="n">
         <v>88</v>
@@ -2901,37 +2946,37 @@
         <v>0</v>
       </c>
       <c r="AG9" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AH9" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AI9" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AJ9" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="AK9" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AL9" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="AM9" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="AN9" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="AO9" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="AP9" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="AQ9" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="AR9" s="0" t="n">
         <v>850</v>
@@ -2940,13 +2985,13 @@
         <v>426</v>
       </c>
       <c r="AT9" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="AU9" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="AV9" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AW9" s="0" t="n">
         <v>14</v>
@@ -2955,7 +3000,7 @@
         <v>10</v>
       </c>
       <c r="AY9" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AZ9" s="0" t="n">
         <v>0</v>
@@ -2964,7 +3009,7 @@
         <v>14</v>
       </c>
       <c r="BB9" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="BC9" s="0" t="n">
         <v>0</v>
@@ -2976,7 +3021,7 @@
         <v>7</v>
       </c>
       <c r="BF9" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2991,19 +3036,19 @@
         <v>98</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>8</v>
@@ -3012,64 +3057,64 @@
         <v>55</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="T10" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="U10" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="V10" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="W10" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="X10" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Y10" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="Z10" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AA10" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB10" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AC10" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AD10" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AE10" s="0" t="n">
         <v>88</v>
@@ -3078,37 +3123,37 @@
         <v>0</v>
       </c>
       <c r="AG10" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AH10" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AI10" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AJ10" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AK10" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AL10" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="AM10" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="AN10" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="AO10" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AP10" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AQ10" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="AR10" s="0" t="n">
         <v>910</v>
@@ -3117,13 +3162,13 @@
         <v>456</v>
       </c>
       <c r="AT10" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="AU10" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="AV10" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AW10" s="0" t="n">
         <v>14</v>
@@ -3132,7 +3177,7 @@
         <v>10</v>
       </c>
       <c r="AY10" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AZ10" s="0" t="n">
         <v>0</v>
@@ -3141,7 +3186,7 @@
         <v>14</v>
       </c>
       <c r="BB10" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="BC10" s="0" t="n">
         <v>0</v>
@@ -3153,7 +3198,7 @@
         <v>8</v>
       </c>
       <c r="BF10" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3168,19 +3213,19 @@
         <v>98</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>8</v>
@@ -3189,64 +3234,64 @@
         <v>55</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="T11" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="U11" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="V11" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="X11" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Y11" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="Z11" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AA11" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB11" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AC11" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AD11" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AE11" s="0" t="n">
         <v>88</v>
@@ -3255,37 +3300,37 @@
         <v>0</v>
       </c>
       <c r="AG11" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AH11" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AI11" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AJ11" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="AK11" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AL11" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="AM11" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="AN11" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="AO11" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="AP11" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="AQ11" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="AR11" s="0" t="n">
         <v>910</v>
@@ -3294,13 +3339,13 @@
         <v>456</v>
       </c>
       <c r="AT11" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="AU11" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="AV11" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AW11" s="0" t="n">
         <v>14</v>
@@ -3309,7 +3354,7 @@
         <v>10</v>
       </c>
       <c r="AY11" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AZ11" s="0" t="n">
         <v>0</v>
@@ -3318,7 +3363,7 @@
         <v>14</v>
       </c>
       <c r="BB11" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="BC11" s="0" t="n">
         <v>0</v>
@@ -3330,7 +3375,7 @@
         <v>8</v>
       </c>
       <c r="BF11" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3345,19 +3390,19 @@
         <v>98</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>8</v>
@@ -3366,64 +3411,64 @@
         <v>55</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Q12" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R12" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="S12" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="T12" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="U12" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="V12" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="W12" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="X12" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Y12" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="Z12" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AA12" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB12" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AC12" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AD12" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AE12" s="0" t="n">
         <v>88</v>
@@ -3432,37 +3477,37 @@
         <v>0</v>
       </c>
       <c r="AG12" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AH12" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AI12" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AJ12" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="AK12" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AL12" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="AM12" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="AN12" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="AO12" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="AP12" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="AQ12" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="AR12" s="0" t="n">
         <v>912</v>
@@ -3471,13 +3516,13 @@
         <v>457</v>
       </c>
       <c r="AT12" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="AU12" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AV12" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AW12" s="0" t="n">
         <v>14</v>
@@ -3486,7 +3531,7 @@
         <v>10</v>
       </c>
       <c r="AY12" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AZ12" s="0" t="n">
         <v>0</v>
@@ -3495,7 +3540,7 @@
         <v>14</v>
       </c>
       <c r="BB12" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="BC12" s="0" t="n">
         <v>0</v>
@@ -3507,7 +3552,7 @@
         <v>8</v>
       </c>
       <c r="BF12" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3522,19 +3567,19 @@
         <v>98</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>8</v>
@@ -3543,64 +3588,64 @@
         <v>55</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Q13" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="S13" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="T13" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="U13" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="V13" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="W13" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="X13" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Y13" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="Z13" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AA13" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AB13" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AC13" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="AD13" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="AE13" s="0" t="n">
         <v>88</v>
@@ -3609,37 +3654,37 @@
         <v>0</v>
       </c>
       <c r="AG13" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AH13" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AI13" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="AJ13" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AK13" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AL13" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AM13" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="AN13" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AO13" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AP13" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AQ13" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AR13" s="0" t="n">
         <v>912</v>
@@ -3648,13 +3693,13 @@
         <v>457</v>
       </c>
       <c r="AT13" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AU13" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="AV13" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AW13" s="0" t="n">
         <v>14</v>
@@ -3663,7 +3708,7 @@
         <v>10</v>
       </c>
       <c r="AY13" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AZ13" s="0" t="n">
         <v>0</v>
@@ -3672,7 +3717,7 @@
         <v>14</v>
       </c>
       <c r="BB13" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="BC13" s="0" t="n">
         <v>0</v>
@@ -3684,7 +3729,7 @@
         <v>8</v>
       </c>
       <c r="BF13" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>